<commit_message>
tugas 3 dan export template
</commit_message>
<xml_diff>
--- a/siper/assets/data/template_data_buku.xlsx
+++ b/siper/assets/data/template_data_buku.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siper\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8890644-1A46-47F0-A322-9AAAAB51AC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB286B-D241-4169-9666-FD066F03480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1E331F79-2C10-49C8-853E-93C1393CF3B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E331F79-2C10-49C8-853E-93C1393CF3B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Buku" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -426,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E7AE47-E912-4C68-BF31-AE187F19B618}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBA92DA-7936-4665-BFFB-6B266AE89D87}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D70327-62D3-4661-A32D-EC94EADA90A9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>